<commit_message>
version with pure recall. behav perf logged at the end.
</commit_message>
<xml_diff>
--- a/stimuli.xlsx
+++ b/stimuli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\pretest_fmri\Guess_fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA4A5B7-DF30-4497-AF10-EE1E3CBE126C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19072BBF-B3C0-4608-8455-1F18B0E00DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1376,9 +1376,6 @@
     <t>folder</t>
   </si>
   <si>
-    <t>pump</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -1559,9 +1556,6 @@
     <t>directory</t>
   </si>
   <si>
-    <t>tire</t>
-  </si>
-  <si>
     <t>ring</t>
   </si>
   <si>
@@ -1859,9 +1853,6 @@
     <t>paper</t>
   </si>
   <si>
-    <t>water</t>
-  </si>
-  <si>
     <t>lock</t>
   </si>
   <si>
@@ -2018,9 +2009,6 @@
     <t>team</t>
   </si>
   <si>
-    <t>gas</t>
-  </si>
-  <si>
     <t>file</t>
   </si>
   <si>
@@ -2130,6 +2118,18 @@
   </si>
   <si>
     <t>dance</t>
+  </si>
+  <si>
+    <t>radio</t>
+  </si>
+  <si>
+    <t>broadcast</t>
+  </si>
+  <si>
+    <t>television</t>
+  </si>
+  <si>
+    <t>music</t>
   </si>
 </sst>
 </file>
@@ -2254,7 +2254,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="41">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2262,314 +2262,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2810,6 +2502,160 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3093,7 +2939,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25"/>
@@ -3173,13 +3019,13 @@
         <v>417</v>
       </c>
       <c r="G2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="I2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -3202,13 +3048,13 @@
         <v>418</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="5"/>
@@ -3230,13 +3076,13 @@
         <v>244</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>245</v>
@@ -3265,13 +3111,13 @@
         <v>419</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>474</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>475</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="1"/>
@@ -3296,13 +3142,13 @@
         <v>420</v>
       </c>
       <c r="G6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H6" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="I6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -3313,7 +3159,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>27</v>
@@ -3325,13 +3171,13 @@
         <v>421</v>
       </c>
       <c r="G7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H7" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="I7" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3354,13 +3200,13 @@
         <v>422</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -3385,13 +3231,13 @@
         <v>423</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -3416,13 +3262,13 @@
         <v>424</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -3447,13 +3293,13 @@
         <v>425</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="1"/>
@@ -3466,7 +3312,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>49</v>
@@ -3478,13 +3324,13 @@
         <v>426</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -3497,7 +3343,7 @@
         <v>55</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>56</v>
@@ -3509,7 +3355,7 @@
         <v>427</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>162</v>
@@ -3537,16 +3383,16 @@
         <v>378</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -3568,16 +3414,16 @@
         <v>223</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="1"/>
@@ -3602,13 +3448,13 @@
         <v>428</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>84</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -3689,7 +3535,7 @@
         <v>203</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>199</v>
@@ -3785,16 +3631,16 @@
         <v>284</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -3900,19 +3746,19 @@
         <v>119</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>266</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>228</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>268</v>
@@ -3943,13 +3789,13 @@
         <v>429</v>
       </c>
       <c r="G27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H27" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="I27" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -3972,13 +3818,13 @@
         <v>430</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -3997,19 +3843,19 @@
         <v>286</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>431</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="1"/>
@@ -4019,28 +3865,28 @@
         <v>185</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>682</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>683</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>686</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="G30" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>689</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>690</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>692</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>693</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="1"/>
@@ -4065,13 +3911,13 @@
         <v>432</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="1"/>
@@ -4084,7 +3930,7 @@
         <v>120</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>300</v>
@@ -4093,16 +3939,16 @@
         <v>301</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="1"/>
@@ -4115,7 +3961,7 @@
         <v>83</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>82</v>
@@ -4127,13 +3973,13 @@
         <v>433</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="1"/>
@@ -4158,13 +4004,13 @@
         <v>434</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>166</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="1"/>
@@ -4189,13 +4035,13 @@
         <v>435</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -4220,13 +4066,13 @@
         <v>436</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -4251,13 +4097,13 @@
         <v>239</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="1"/>
@@ -4282,13 +4128,13 @@
         <v>437</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="1"/>
@@ -4313,13 +4159,13 @@
         <v>438</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -4344,13 +4190,13 @@
         <v>439</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -4366,7 +4212,7 @@
         <v>290</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>291</v>
@@ -4375,13 +4221,13 @@
         <v>236</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="1"/>
@@ -4406,13 +4252,13 @@
         <v>440</v>
       </c>
       <c r="G42" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H42" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="I42" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -4420,28 +4266,28 @@
         <v>184</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>164</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -4466,13 +4312,13 @@
         <v>441</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="1"/>
@@ -4497,13 +4343,13 @@
         <v>442</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="1"/>
@@ -4513,7 +4359,7 @@
         <v>184</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>375</v>
@@ -4525,13 +4371,13 @@
         <v>376</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>267</v>
@@ -4559,13 +4405,13 @@
         <v>443</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="1"/>
@@ -4590,13 +4436,13 @@
         <v>444</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -4606,28 +4452,28 @@
         <v>184</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>445</v>
+        <v>693</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>506</v>
+        <v>694</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>659</v>
+        <v>695</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>606</v>
+        <v>696</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -4649,16 +4495,16 @@
         <v>330</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -4671,7 +4517,7 @@
         <v>130</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>332</v>
@@ -4680,16 +4526,16 @@
         <v>331</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="1"/>
@@ -4711,16 +4557,16 @@
         <v>334</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="1"/>
@@ -4736,22 +4582,22 @@
         <v>15</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>28</v>
       </c>
       <c r="F53" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G53" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H53" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="I53" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -4762,7 +4608,7 @@
         <v>68</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>69</v>
@@ -4771,16 +4617,16 @@
         <v>70</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
@@ -4802,16 +4648,16 @@
         <v>335</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -4833,16 +4679,16 @@
         <v>338</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="1"/>
@@ -4864,16 +4710,16 @@
         <v>341</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -4889,19 +4735,19 @@
         <v>109</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>343</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>185</v>
@@ -4926,16 +4772,16 @@
         <v>344</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="1"/>
@@ -4948,25 +4794,25 @@
         <v>16</v>
       </c>
       <c r="C60" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>651</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>654</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F60" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G60" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="H60" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="I60" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -4986,16 +4832,16 @@
         <v>349</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -5017,16 +4863,16 @@
         <v>303</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>160</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -5048,16 +4894,16 @@
         <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G63" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H63" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I63" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -5080,13 +4926,13 @@
         <v>235</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="J64" s="3"/>
       <c r="K64" s="1"/>
@@ -5108,16 +4954,16 @@
         <v>352</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="J65" s="3"/>
       <c r="K65" s="1"/>
@@ -5136,19 +4982,19 @@
         <v>354</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="J66" s="3"/>
       <c r="K66" s="1"/>
@@ -5170,16 +5016,16 @@
         <v>299</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="5"/>
@@ -5192,7 +5038,7 @@
         <v>3</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>17</v>
@@ -5201,16 +5047,16 @@
         <v>18</v>
       </c>
       <c r="F68" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G68" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="H68" t="s">
+        <v>565</v>
+      </c>
+      <c r="I68" t="s">
         <v>567</v>
-      </c>
-      <c r="I68" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -5221,7 +5067,7 @@
         <v>37</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>38</v>
@@ -5230,16 +5076,16 @@
         <v>39</v>
       </c>
       <c r="F69" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G69" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="H69" t="s">
+        <v>566</v>
+      </c>
+      <c r="I69" t="s">
         <v>568</v>
-      </c>
-      <c r="I69" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -5259,16 +5105,16 @@
         <v>47</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G70" s="9" t="s">
         <v>439</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
@@ -5290,16 +5136,16 @@
         <v>54</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
@@ -5322,16 +5168,16 @@
         <v>359</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="J72" s="3"/>
       <c r="K72" s="1"/>
@@ -5353,16 +5199,16 @@
         <v>362</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -5381,7 +5227,7 @@
         <v>365</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>403</v>
@@ -5393,7 +5239,7 @@
         <v>405</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="J74" s="3"/>
       <c r="K74" s="1"/>
@@ -5449,7 +5295,7 @@
         <v>406</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>407</v>
@@ -5496,10 +5342,10 @@
         <v>148</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>367</v>
@@ -5517,7 +5363,7 @@
         <v>398</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="J78" s="3"/>
       <c r="K78" s="1"/>
@@ -5570,10 +5416,10 @@
         <v>138</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H80" s="5" t="s">
         <v>416</v>
@@ -5592,7 +5438,7 @@
         <v>129</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>318</v>
@@ -5601,7 +5447,7 @@
         <v>287</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>275</v>
@@ -5665,61 +5511,61 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:A81 A86:A89">
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
       <formula>"plant"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
       <formula>"abstract"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A81 A86:A90">
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
       <formula>"person"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>"animal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A89">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"location"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A90">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"food"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82 B1:E10 B12:E81 B11:D11">
-    <cfRule type="duplicateValues" dxfId="26" priority="163"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="163"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86:B89 A90:A91 A104:A1048576 B1:B82">
-    <cfRule type="duplicateValues" dxfId="25" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90:B91 C1:C7 C9:C81 C86:C89 B104:B1048576 C8:D8">
-    <cfRule type="duplicateValues" dxfId="23" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:E1048576">
+    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E81">
-    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86:E89 A90:E91 A104:E1048576 C92:E103 B82 B1:E10 B12:E81 B11:D11">
-    <cfRule type="duplicateValues" dxfId="21" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:C1048576 D1:D7 D9:D81 D86:D89">
-    <cfRule type="duplicateValues" dxfId="20" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D90:D1048576 E1:E10 E86:E89 E12:E81">
-    <cfRule type="duplicateValues" dxfId="19" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90:E1048576">
-    <cfRule type="duplicateValues" dxfId="18" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:I1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5868,7 +5714,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="56" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6124,23 +5970,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="55" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="54" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:F1">
-    <cfRule type="duplicateValues" dxfId="53" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="duplicateValues" dxfId="52" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="duplicateValues" dxfId="51" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="duplicateValues" dxfId="50" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6223,44 +6069,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="48" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="47" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="46" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="45" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="44" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="43" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="42" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="41" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:B4">
-    <cfRule type="duplicateValues" dxfId="40" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:B5">
-    <cfRule type="duplicateValues" dxfId="39" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6">
-    <cfRule type="duplicateValues" dxfId="38" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B7">
-    <cfRule type="duplicateValues" dxfId="37" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="36" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="35" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="34" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>